<commit_message>
Atualização de todas as pastas
</commit_message>
<xml_diff>
--- a/Indice .xlsx
+++ b/Indice .xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7965" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="ORDEM ALFABETICA" sheetId="1" r:id="rId1"/>
     <sheet name="ORDEM NUMERICA" sheetId="4" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="85">
   <si>
     <t>Índice</t>
   </si>
@@ -27,19 +26,19 @@
     <t>Oh quão lindo esse nome é</t>
   </si>
   <si>
-    <t>Acredito</t>
-  </si>
-  <si>
-    <t>Oh Senhor</t>
+    <t>Algo novo</t>
+  </si>
+  <si>
+    <t>Ousado amor</t>
   </si>
   <si>
     <t>Aliança de sangue</t>
   </si>
   <si>
-    <t>Ousado amor</t>
-  </si>
-  <si>
-    <t>Alicança</t>
+    <t>Pedra preciosa</t>
+  </si>
+  <si>
+    <t>Ambiente de glória</t>
   </si>
   <si>
     <t>Perto quero estar</t>
@@ -63,21 +62,21 @@
     <t>Pra sempre</t>
   </si>
   <si>
+    <t>Aquieta minh'alma</t>
+  </si>
+  <si>
+    <t>Primeira essência</t>
+  </si>
+  <si>
     <t>Beija-me com tua glória</t>
   </si>
   <si>
-    <t>Primeira essência</t>
+    <t>Quando o vento soprar</t>
   </si>
   <si>
     <t>Caia fogo</t>
   </si>
   <si>
-    <t>Quando o vento soprar</t>
-  </si>
-  <si>
-    <t>Caminho no deserto</t>
-  </si>
-  <si>
     <t>Quanto mais eu te buscar</t>
   </si>
   <si>
@@ -87,37 +86,37 @@
     <t>Quão formoso</t>
   </si>
   <si>
-    <t>Casa do Pai</t>
+    <t>Ceu e terra</t>
+  </si>
+  <si>
+    <t>Que amor é esse</t>
+  </si>
+  <si>
+    <t>Cobre-me</t>
   </si>
   <si>
     <t>Queima de novo</t>
   </si>
   <si>
-    <t>Ceu e terra</t>
-  </si>
-  <si>
-    <t>Questiona  ou adora</t>
-  </si>
-  <si>
-    <t>Cobre-me</t>
+    <t>Coração igual ao teu</t>
   </si>
   <si>
     <t>Ressuscitou</t>
   </si>
   <si>
-    <t>Coração igual ao teu</t>
+    <t>Cria em mim</t>
   </si>
   <si>
     <t>Senhor te quero</t>
   </si>
   <si>
-    <t>Cria em mim</t>
+    <t>Cristo vive em mim</t>
   </si>
   <si>
     <t>Ser conhecido de Deus</t>
   </si>
   <si>
-    <t>Cristo vive em mim</t>
+    <t>Digno</t>
   </si>
   <si>
     <t>Seu sangue</t>
@@ -126,7 +125,7 @@
     <t>Digno de Gloria</t>
   </si>
   <si>
-    <t>Só em ti confiarei</t>
+    <t>Sinto fluir</t>
   </si>
   <si>
     <t>Ele vem</t>
@@ -138,16 +137,16 @@
     <t>Em espirito, em verdade</t>
   </si>
   <si>
+    <t>Som do ceu</t>
+  </si>
+  <si>
+    <t>Em teus braços</t>
+  </si>
+  <si>
     <t>Sonda-me ho Deus</t>
   </si>
   <si>
-    <t>Em teus braços</t>
-  </si>
-  <si>
-    <t>Sonda-me Senhor</t>
-  </si>
-  <si>
-    <t>Em ti esperarei</t>
+    <t>Emaús</t>
   </si>
   <si>
     <t>Sou humano</t>
@@ -159,7 +158,7 @@
     <t>Sou teu</t>
   </si>
   <si>
-    <t>És meu Deus</t>
+    <t>Essência da adoração</t>
   </si>
   <si>
     <t>Teu amor não falha</t>
@@ -174,16 +173,16 @@
     <t>Eu navegarei</t>
   </si>
   <si>
-    <t>Teu santo nome</t>
-  </si>
-  <si>
-    <t>Extraordinário</t>
-  </si>
-  <si>
-    <t>Todas as coisas</t>
-  </si>
-  <si>
-    <t>Fala comigo</t>
+    <t>Teu reino me chamou de seu</t>
+  </si>
+  <si>
+    <t>Eu vou construir</t>
+  </si>
+  <si>
+    <t>Tua alegria</t>
+  </si>
+  <si>
+    <t>Filho do Deus vivo</t>
   </si>
   <si>
     <t>Tua graça me basta</t>
@@ -195,115 +194,82 @@
     <t>Tua palavra</t>
   </si>
   <si>
+    <t>Grande é o senhor</t>
+  </si>
+  <si>
+    <t>Uma coisa peço ao Senhor</t>
+  </si>
+  <si>
     <t>Há um lugar</t>
   </si>
   <si>
+    <t>Venha o teu reino</t>
+  </si>
+  <si>
+    <t>Hosana</t>
+  </si>
+  <si>
     <t>Vim para adorar-te</t>
   </si>
   <si>
-    <t>Hosana</t>
+    <t>Infinitamente mais</t>
+  </si>
+  <si>
+    <t>Vou deixar na cruz</t>
+  </si>
+  <si>
+    <t>Invocamos</t>
   </si>
   <si>
     <t>Yeshua</t>
   </si>
   <si>
-    <t>Infinitamente mais</t>
-  </si>
-  <si>
-    <t>invocamos</t>
-  </si>
-  <si>
     <t>Jesus é o caminho</t>
   </si>
   <si>
+    <t>Jesus em tua presença</t>
+  </si>
+  <si>
     <t>Lembra Senhor</t>
   </si>
   <si>
-    <t>Leva-me a cruz</t>
-  </si>
-  <si>
     <t>Lugar secreto</t>
   </si>
   <si>
     <t>Lugar seguro</t>
   </si>
   <si>
-    <t>Manancial</t>
-  </si>
-  <si>
     <t>Me faz te conhecer</t>
   </si>
   <si>
+    <t>Me leva o deserto</t>
+  </si>
+  <si>
+    <t>Melhor lugar</t>
+  </si>
+  <si>
     <t>Meu alvo</t>
   </si>
   <si>
-    <t>Meu universo</t>
-  </si>
-  <si>
     <t>Mil graus</t>
   </si>
   <si>
     <t>Mostra-me tua face</t>
   </si>
   <si>
-    <t>Muda minha vida</t>
-  </si>
-  <si>
     <t>Nada alem do sangue</t>
   </si>
   <si>
     <t>Não há Deus maior</t>
   </si>
   <si>
+    <t>Não há um nome igual</t>
+  </si>
+  <si>
     <t>No caminho do milagre</t>
   </si>
   <si>
-    <t>O que fazer quando Ele vem</t>
-  </si>
-  <si>
     <t>Oceanos</t>
-  </si>
-  <si>
-    <t>Digno</t>
-  </si>
-  <si>
-    <t>Me leva o deserto</t>
-  </si>
-  <si>
-    <t>Filho do Deus vivo</t>
-  </si>
-  <si>
-    <t>Essência da adoração</t>
-  </si>
-  <si>
-    <t>Vou deixar na cruz</t>
-  </si>
-  <si>
-    <t>Pedra preciosa</t>
-  </si>
-  <si>
-    <t>Algo novo</t>
-  </si>
-  <si>
-    <t>Jesus em tua presença</t>
-  </si>
-  <si>
-    <t>Emaús</t>
-  </si>
-  <si>
-    <t>Que amor é esse</t>
-  </si>
-  <si>
-    <t>Eu vou construir</t>
-  </si>
-  <si>
-    <t>Ambiente de glória</t>
-  </si>
-  <si>
-    <t>Não há um nome igual</t>
-  </si>
-  <si>
-    <t>Grande é o senhor</t>
   </si>
 </sst>
 </file>
@@ -311,10 +277,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -368,36 +334,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,6 +348,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -419,9 +378,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,7 +409,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,23 +469,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -533,12 +499,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -551,7 +511,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,13 +577,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,25 +589,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,25 +607,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,7 +643,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,55 +673,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,26 +721,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -801,6 +747,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,149 +824,149 @@
     <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1023,20 +989,20 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1051,6 +1017,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1406,8 +1373,8 @@
   <sheetPr/>
   <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -1444,7 +1411,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" ht="14.1" customHeight="1" spans="1:5">
+    <row r="3" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A3" s="7">
         <v>46</v>
       </c>
@@ -1459,22 +1426,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="14.1" customHeight="1" spans="1:5">
+    <row r="4" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A4" s="7">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="7">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" ht="14.1" customHeight="1" spans="1:5">
+    <row r="5" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A5" s="7">
         <v>26</v>
       </c>
@@ -1483,15 +1450,15 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="7">
-        <v>68</v>
-      </c>
-      <c r="E5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="14.1" customHeight="1" spans="1:5">
+    <row r="6" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A6" s="7">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>7</v>
@@ -1504,7 +1471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" ht="14.1" customHeight="1" spans="1:5">
+    <row r="7" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A7" s="7">
         <v>60</v>
       </c>
@@ -1519,7 +1486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" ht="14.1" customHeight="1" spans="1:5">
+    <row r="8" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A8" s="7">
         <v>12</v>
       </c>
@@ -1534,7 +1501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" ht="14.1" customHeight="1" spans="1:5">
+    <row r="9" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -1549,9 +1516,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="14.1" customHeight="1" spans="1:5">
+    <row r="10" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A10" s="7">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>15</v>
@@ -1564,9 +1531,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" ht="14.1" customHeight="1" spans="1:5">
+    <row r="11" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A11" s="7">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>17</v>
@@ -1579,9 +1546,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" ht="14.1" customHeight="1" spans="1:5">
+    <row r="12" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A12" s="7">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>19</v>
@@ -1594,7 +1561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" ht="14.1" customHeight="1" spans="1:5">
+    <row r="13" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A13" s="7">
         <v>65</v>
       </c>
@@ -1609,39 +1576,39 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" ht="14.1" customHeight="1" spans="1:5">
+    <row r="14" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A14" s="7">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="7">
-        <v>78</v>
-      </c>
-      <c r="E14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" ht="14.1" customHeight="1" spans="1:5">
+    <row r="15" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A15" s="7">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="7">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" ht="14.1" customHeight="1" spans="1:5">
+    <row r="16" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A16" s="7">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>27</v>
@@ -1654,9 +1621,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" ht="14.1" customHeight="1" spans="1:5">
+    <row r="17" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A17" s="7">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>29</v>
@@ -1669,9 +1636,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" ht="14.1" customHeight="1" spans="1:5">
+    <row r="18" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A18" s="7">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>31</v>
@@ -1680,13 +1647,13 @@
       <c r="D18" s="7">
         <v>79</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" ht="14.1" customHeight="1" spans="1:5">
+    <row r="19" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A19" s="7">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>33</v>
@@ -1699,7 +1666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" ht="14.1" customHeight="1" spans="1:5">
+    <row r="20" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A20" s="7">
         <v>23</v>
       </c>
@@ -1708,13 +1675,13 @@
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="7">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" ht="14.1" customHeight="1" spans="1:5">
+    <row r="21" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -1725,11 +1692,11 @@
       <c r="D21" s="7">
         <v>76</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" ht="14.1" customHeight="1" spans="1:5">
+    <row r="22" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A22" s="7">
         <v>20</v>
       </c>
@@ -1738,13 +1705,13 @@
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="7">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" ht="14.1" customHeight="1" spans="1:5">
+    <row r="23" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A23" s="7">
         <v>5</v>
       </c>
@@ -1753,15 +1720,15 @@
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="7">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" ht="14.1" customHeight="1" spans="1:5">
+    <row r="24" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A24" s="7">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>43</v>
@@ -1774,7 +1741,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" ht="14.1" customHeight="1" spans="1:5">
+    <row r="25" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A25" s="7">
         <v>63</v>
       </c>
@@ -1785,13 +1752,13 @@
       <c r="D25" s="7">
         <v>67</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" ht="14.1" customHeight="1" spans="1:5">
+    <row r="26" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A26" s="7">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>47</v>
@@ -1804,11 +1771,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" ht="14.1" customHeight="1" spans="1:5">
+    <row r="27" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A27" s="7">
         <v>74</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="9"/>
@@ -1819,7 +1786,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" ht="14.1" customHeight="1" spans="1:5">
+    <row r="28" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A28" s="7">
         <v>14</v>
       </c>
@@ -1830,26 +1797,26 @@
       <c r="D28" s="7">
         <v>72</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" ht="14.1" customHeight="1" spans="1:5">
+    <row r="29" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A29" s="7">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="7">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" ht="14.1" customHeight="1" spans="1:5">
+    <row r="30" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A30" s="7">
         <v>18</v>
       </c>
@@ -1864,7 +1831,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" ht="14.1" customHeight="1" spans="1:5">
+    <row r="31" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A31" s="7">
         <v>55</v>
       </c>
@@ -1879,285 +1846,261 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" ht="14.1" customHeight="1" spans="1:5">
+    <row r="32" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A32" s="7">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="7">
-        <v>75</v>
-      </c>
-      <c r="E32" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" ht="14.1" customHeight="1" spans="1:5">
+    <row r="33" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A33" s="7">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="7">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" ht="14.1" customHeight="1" spans="1:5">
+    <row r="34" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A34" s="7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="7">
-        <v>82</v>
-      </c>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" ht="14.1" customHeight="1" spans="1:5">
+        <v>75</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A35" s="7">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="7">
-        <v>83</v>
-      </c>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" ht="14.1" customHeight="1" spans="1:5">
+        <v>29</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A36" s="7">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="7">
-        <v>84</v>
-      </c>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" ht="14.1" customHeight="1" spans="1:5">
+        <v>40</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A37" s="7">
+        <v>62</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A38" s="7">
+        <v>42</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+    </row>
+    <row r="39" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A39" s="7">
         <v>81</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="7">
-        <v>85</v>
-      </c>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A38" s="7">
-        <v>51</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="7">
-        <v>86</v>
-      </c>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A39" s="7">
+      <c r="B39" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A40" s="7">
         <v>69</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="7">
-        <v>87</v>
-      </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A40" s="7">
+      <c r="B40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A41" s="7">
         <v>44</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="7">
-        <v>88</v>
-      </c>
-      <c r="E40" s="11"/>
-    </row>
-    <row r="41" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A41" s="7">
-        <v>29</v>
-      </c>
       <c r="B41" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C41" s="9"/>
-      <c r="D41" s="7">
-        <v>89</v>
-      </c>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" ht="14.1" customHeight="1" spans="1:5">
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A42" s="7">
         <v>25</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C42" s="9"/>
-      <c r="D42" s="7">
-        <v>90</v>
-      </c>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" ht="14.1" customHeight="1" spans="1:5">
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+    </row>
+    <row r="43" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A43" s="7">
+        <v>8</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+    </row>
+    <row r="44" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A44" s="7">
+        <v>82</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+    </row>
+    <row r="45" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A45" s="7">
         <v>41</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="7">
-        <v>91</v>
-      </c>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A44" s="7">
-        <v>57</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="7">
-        <v>92</v>
-      </c>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A45" s="7">
+      <c r="B45" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+    </row>
+    <row r="46" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A46" s="7">
         <v>70</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="7">
-        <v>93</v>
-      </c>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A46" s="7">
+      <c r="B46" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+    </row>
+    <row r="47" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A47" s="7">
         <v>66</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="7">
-        <v>94</v>
-      </c>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A47" s="7">
-        <v>80</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>76</v>
+      <c r="B47" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C47" s="9"/>
-      <c r="D47" s="7">
-        <v>95</v>
-      </c>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" ht="14.1" customHeight="1" spans="1:5">
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+    </row>
+    <row r="48" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A48" s="7">
         <v>59</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C48" s="9"/>
-      <c r="D48" s="7">
-        <v>96</v>
-      </c>
-      <c r="E48" s="11"/>
-    </row>
-    <row r="49" ht="14.1" customHeight="1" spans="1:5">
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+    </row>
+    <row r="49" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A49" s="7">
         <v>30</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C49" s="9"/>
-      <c r="D49" s="7">
-        <v>97</v>
-      </c>
-      <c r="E49" s="12"/>
-    </row>
-    <row r="50" ht="14.1" customHeight="1" spans="1:5">
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+    </row>
+    <row r="50" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A50" s="7">
+        <v>56</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+    </row>
+    <row r="51" customFormat="1" ht="14" customHeight="1" spans="1:5">
+      <c r="A51" s="7">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="7">
-        <v>98</v>
-      </c>
-      <c r="E50" s="10"/>
-    </row>
-    <row r="51" ht="14.1" customHeight="1" spans="1:5">
-      <c r="A51" s="7">
-        <v>77</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>80</v>
+      <c r="B51" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="C51" s="9"/>
-      <c r="D51" s="7">
-        <v>99</v>
-      </c>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" ht="14.1" customHeight="1" spans="1:5">
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+    </row>
+    <row r="52" customFormat="1" ht="14" customHeight="1" spans="1:5">
       <c r="A52" s="7">
         <v>73</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>81</v>
+      <c r="B52" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="7">
-        <v>100</v>
-      </c>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" ht="14.1" customHeight="1" spans="3:3">
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+    </row>
+    <row r="53" ht="14.1" customHeight="1" spans="3:5">
       <c r="C53" s="13"/>
+      <c r="D53"/>
+      <c r="E53"/>
     </row>
     <row r="54" ht="14.1" customHeight="1" spans="3:3">
       <c r="C54" s="13"/>
@@ -2924,8 +2867,8 @@
       <c r="E195" s="14"/>
     </row>
   </sheetData>
-  <sortState ref="A1:E102">
-    <sortCondition ref="B67"/>
+  <sortState ref="A3:B86">
+    <sortCondition ref="B3:B86"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:E2"/>
@@ -2941,8 +2884,8 @@
   <sheetPr/>
   <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A52" sqref="$A1:$XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -2979,22 +2922,22 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" ht="14.1" customHeight="1" spans="1:5">
+    <row r="3" ht="14" customHeight="1" spans="1:5">
       <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="7">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="14.1" customHeight="1" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" ht="14" customHeight="1" spans="1:5">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -3003,13 +2946,13 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="7">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" ht="14.1" customHeight="1" spans="1:5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" ht="14" customHeight="1" spans="1:5">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -3018,28 +2961,28 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="7">
-        <v>68</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" ht="14.1" customHeight="1" spans="1:5">
+        <v>53</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" ht="14" customHeight="1" spans="1:5">
       <c r="A6" s="7">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="7">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" ht="14.1" customHeight="1" spans="1:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" ht="14" customHeight="1" spans="1:5">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -3048,58 +2991,58 @@
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="7">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" ht="14.1" customHeight="1" spans="1:5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" ht="14" customHeight="1" spans="1:5">
       <c r="A8" s="7">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="7">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" ht="14.1" customHeight="1" spans="1:5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" ht="14" customHeight="1" spans="1:5">
       <c r="A9" s="7">
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="7">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" ht="14.1" customHeight="1" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" ht="14" customHeight="1" spans="1:5">
       <c r="A10" s="7">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="7">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" ht="14.1" customHeight="1" spans="1:5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" ht="14" customHeight="1" spans="1:5">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -3108,13 +3051,13 @@
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="7">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" ht="14.1" customHeight="1" spans="1:5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" ht="14" customHeight="1" spans="1:5">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -3123,13 +3066,13 @@
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="7">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" ht="14.1" customHeight="1" spans="1:5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" ht="14" customHeight="1" spans="1:5">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -3138,13 +3081,13 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="7">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" ht="14.1" customHeight="1" spans="1:5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" ht="14" customHeight="1" spans="1:5">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -3153,13 +3096,13 @@
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="7">
-        <v>78</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" ht="14.1" customHeight="1" spans="1:5">
+        <v>62</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" ht="14" customHeight="1" spans="1:5">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -3168,13 +3111,13 @@
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="7">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" ht="14.1" customHeight="1" spans="1:5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" ht="14" customHeight="1" spans="1:5">
       <c r="A16" s="7">
         <v>14</v>
       </c>
@@ -3183,13 +3126,13 @@
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="7">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" ht="14.1" customHeight="1" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" ht="14" customHeight="1" spans="1:5">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -3198,58 +3141,58 @@
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="7">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" ht="14.1" customHeight="1" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" ht="14" customHeight="1" spans="1:5">
       <c r="A18" s="7">
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="7">
+        <v>66</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" ht="14.1" customHeight="1" spans="1:5">
+    </row>
+    <row r="19" ht="14" customHeight="1" spans="1:5">
       <c r="A19" s="7">
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="7">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" ht="14.1" customHeight="1" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" ht="14" customHeight="1" spans="1:5">
       <c r="A20" s="7">
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="7">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" ht="14.1" customHeight="1" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" ht="14" customHeight="1" spans="1:5">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -3258,13 +3201,13 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="7">
-        <v>76</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" ht="14.1" customHeight="1" spans="1:5">
+        <v>69</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" ht="14" customHeight="1" spans="1:5">
       <c r="A22" s="7">
         <v>20</v>
       </c>
@@ -3273,43 +3216,43 @@
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="7">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" ht="14.1" customHeight="1" spans="1:5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" ht="14" customHeight="1" spans="1:5">
       <c r="A23" s="7">
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="7">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" ht="14.1" customHeight="1" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" ht="14" customHeight="1" spans="1:5">
       <c r="A24" s="7">
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="7">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" ht="14.1" customHeight="1" spans="1:5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" ht="14" customHeight="1" spans="1:5">
       <c r="A25" s="7">
         <v>23</v>
       </c>
@@ -3318,13 +3261,13 @@
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="7">
-        <v>67</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" ht="14.1" customHeight="1" spans="1:5">
+        <v>73</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" ht="14" customHeight="1" spans="1:5">
       <c r="A26" s="7">
         <v>24</v>
       </c>
@@ -3333,28 +3276,28 @@
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="7">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" ht="14.1" customHeight="1" spans="1:5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" ht="14" customHeight="1" spans="1:5">
       <c r="A27" s="7">
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="7">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" ht="14.1" customHeight="1" spans="1:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" ht="14" customHeight="1" spans="1:5">
       <c r="A28" s="7">
         <v>26</v>
       </c>
@@ -3363,73 +3306,73 @@
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="7">
-        <v>72</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" ht="14.1" customHeight="1" spans="1:5">
+        <v>76</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" ht="14" customHeight="1" spans="1:5">
       <c r="A29" s="7">
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="7">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" ht="14.1" customHeight="1" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" ht="14" customHeight="1" spans="1:5">
       <c r="A30" s="7">
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="7">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" ht="14.1" customHeight="1" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" ht="14" customHeight="1" spans="1:5">
       <c r="A31" s="7">
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="7">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" ht="14.1" customHeight="1" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" ht="14" customHeight="1" spans="1:5">
       <c r="A32" s="7">
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="7">
-        <v>75</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" ht="14.1" customHeight="1" spans="1:5">
+        <v>80</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" ht="14" customHeight="1" spans="1:5">
       <c r="A33" s="7">
         <v>31</v>
       </c>
@@ -3438,13 +3381,13 @@
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="7">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" ht="14.1" customHeight="1" spans="1:5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" ht="14" customHeight="1" spans="1:5">
       <c r="A34" s="7">
         <v>32</v>
       </c>
@@ -3455,22 +3398,26 @@
       <c r="D34" s="7">
         <v>82</v>
       </c>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E34" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" ht="14" customHeight="1" spans="1:5">
       <c r="A35" s="7">
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="7">
         <v>83</v>
       </c>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E35" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" ht="14" customHeight="1" spans="1:5">
       <c r="A36" s="7">
         <v>34</v>
       </c>
@@ -3481,22 +3428,24 @@
       <c r="D36" s="7">
         <v>84</v>
       </c>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E36" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" ht="14" customHeight="1" spans="1:5">
       <c r="A37" s="7">
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="7">
         <v>85</v>
       </c>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" ht="14" customHeight="1" spans="1:5">
       <c r="A38" s="7">
         <v>36</v>
       </c>
@@ -3507,9 +3456,9 @@
       <c r="D38" s="7">
         <v>86</v>
       </c>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" ht="14" customHeight="1" spans="1:5">
       <c r="A39" s="7">
         <v>37</v>
       </c>
@@ -3520,9 +3469,9 @@
       <c r="D39" s="7">
         <v>87</v>
       </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" ht="14" customHeight="1" spans="1:5">
       <c r="A40" s="7">
         <v>38</v>
       </c>
@@ -3533,61 +3482,61 @@
       <c r="D40" s="7">
         <v>88</v>
       </c>
-      <c r="E40" s="11"/>
-    </row>
-    <row r="41" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" ht="14" customHeight="1" spans="1:5">
       <c r="A41" s="7">
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="7">
         <v>89</v>
       </c>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" ht="14" customHeight="1" spans="1:5">
       <c r="A42" s="7">
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="7">
         <v>90</v>
       </c>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" ht="14" customHeight="1" spans="1:5">
       <c r="A43" s="7">
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="7">
         <v>91</v>
       </c>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" ht="14" customHeight="1" spans="1:5">
       <c r="A44" s="7">
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="7">
         <v>92</v>
       </c>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" ht="14" customHeight="1" spans="1:5">
       <c r="A45" s="7">
         <v>43</v>
       </c>
@@ -3598,35 +3547,35 @@
       <c r="D45" s="7">
         <v>93</v>
       </c>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" ht="14" customHeight="1" spans="1:5">
       <c r="A46" s="7">
         <v>44</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="7">
         <v>94</v>
       </c>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" ht="14" customHeight="1" spans="1:5">
       <c r="A47" s="7">
         <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="7">
         <v>95</v>
       </c>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" ht="14" customHeight="1" spans="1:5">
       <c r="A48" s="7">
         <v>46</v>
       </c>
@@ -3637,22 +3586,22 @@
       <c r="D48" s="7">
         <v>96</v>
       </c>
-      <c r="E48" s="11"/>
-    </row>
-    <row r="49" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" ht="14" customHeight="1" spans="1:5">
       <c r="A49" s="7">
         <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="7">
         <v>97</v>
       </c>
-      <c r="E49" s="12"/>
-    </row>
-    <row r="50" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" ht="14" customHeight="1" spans="1:5">
       <c r="A50" s="7">
         <v>48</v>
       </c>
@@ -3663,320 +3612,134 @@
       <c r="D50" s="7">
         <v>98</v>
       </c>
-      <c r="E50" s="10"/>
-    </row>
-    <row r="51" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" ht="14" customHeight="1" spans="1:5">
       <c r="A51" s="7">
         <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="7">
         <v>99</v>
       </c>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" ht="14.1" customHeight="1" spans="1:5">
+      <c r="E51" s="11"/>
+    </row>
+    <row r="52" ht="14" customHeight="1" spans="1:5">
       <c r="A52" s="7">
         <v>50</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="7">
         <v>100</v>
       </c>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A53" s="7">
-        <v>51</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>92</v>
-      </c>
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" ht="14" customHeight="1" spans="3:3">
       <c r="C53" s="13"/>
     </row>
-    <row r="54" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A54" s="7">
-        <v>52</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>59</v>
-      </c>
+    <row r="54" ht="14" customHeight="1" spans="3:3">
       <c r="C54" s="13"/>
     </row>
-    <row r="55" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A55" s="7">
-        <v>53</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>93</v>
-      </c>
+    <row r="55" ht="14" customHeight="1" spans="3:3">
       <c r="C55" s="13"/>
     </row>
-    <row r="56" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A56" s="7">
-        <v>54</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>17</v>
-      </c>
+    <row r="56" ht="14" customHeight="1" spans="3:3">
       <c r="C56" s="13"/>
     </row>
-    <row r="57" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A57" s="7">
-        <v>55</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>57</v>
-      </c>
+    <row r="57" ht="14" customHeight="1" spans="3:3">
       <c r="C57" s="13"/>
     </row>
-    <row r="58" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A58" s="7">
-        <v>56</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>94</v>
-      </c>
+    <row r="58" ht="14" customHeight="1" spans="3:3">
       <c r="C58" s="13"/>
     </row>
-    <row r="59" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A59" s="7">
-        <v>57</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>95</v>
-      </c>
+    <row r="59" ht="14" customHeight="1" spans="3:3">
       <c r="C59" s="13"/>
     </row>
-    <row r="60" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A60" s="7">
-        <v>58</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>50</v>
-      </c>
+    <row r="60" ht="14" customHeight="1" spans="3:3">
       <c r="C60" s="13"/>
     </row>
-    <row r="61" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A61" s="7">
-        <v>59</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>77</v>
-      </c>
+    <row r="61" ht="14" customHeight="1" spans="3:3">
       <c r="C61" s="13"/>
     </row>
-    <row r="62" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A62" s="7">
-        <v>60</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>9</v>
-      </c>
+    <row r="62" ht="14" customHeight="1" spans="3:3">
       <c r="C62" s="13"/>
     </row>
-    <row r="63" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A63" s="7">
-        <v>61</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>26</v>
-      </c>
+    <row r="63" ht="14" customHeight="1" spans="3:3">
       <c r="C63" s="14"/>
     </row>
-    <row r="64" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A64" s="7">
-        <v>62</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>65</v>
-      </c>
+    <row r="64" ht="14" customHeight="1" spans="3:3">
       <c r="C64" s="14"/>
     </row>
-    <row r="65" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A65" s="7">
-        <v>63</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>45</v>
-      </c>
+    <row r="65" ht="14" customHeight="1" spans="3:3">
       <c r="C65" s="14"/>
     </row>
-    <row r="66" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A66" s="7">
-        <v>64</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>2</v>
-      </c>
+    <row r="66" ht="14" customHeight="1" spans="3:3">
       <c r="C66" s="14"/>
     </row>
-    <row r="67" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A67" s="7">
-        <v>65</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>21</v>
-      </c>
+    <row r="67" ht="14" customHeight="1" spans="3:3">
       <c r="C67" s="14"/>
     </row>
-    <row r="68" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A68" s="7">
-        <v>66</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>75</v>
-      </c>
+    <row r="68" ht="14" customHeight="1" spans="3:3">
       <c r="C68" s="14"/>
     </row>
-    <row r="69" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A69" s="7">
-        <v>67</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>46</v>
-      </c>
+    <row r="69" ht="14" customHeight="1" spans="3:3">
       <c r="C69" s="14"/>
     </row>
-    <row r="70" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A70" s="7">
-        <v>68</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>6</v>
-      </c>
+    <row r="70" ht="14" customHeight="1" spans="3:3">
       <c r="C70" s="14"/>
     </row>
-    <row r="71" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A71" s="7">
-        <v>69</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>68</v>
-      </c>
+    <row r="71" ht="14" customHeight="1" spans="3:3">
       <c r="C71" s="14"/>
     </row>
-    <row r="72" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A72" s="7">
-        <v>70</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>74</v>
-      </c>
+    <row r="72" ht="14" customHeight="1" spans="3:3">
       <c r="C72" s="14"/>
     </row>
-    <row r="73" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A73" s="7">
-        <v>71</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>36</v>
-      </c>
+    <row r="73" ht="14" customHeight="1" spans="3:3">
       <c r="C73" s="14"/>
     </row>
-    <row r="74" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A74" s="7">
-        <v>72</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>52</v>
-      </c>
+    <row r="74" ht="14" customHeight="1" spans="3:3">
       <c r="C74" s="14"/>
     </row>
-    <row r="75" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A75" s="7">
-        <v>73</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>81</v>
-      </c>
+    <row r="75" ht="14" customHeight="1" spans="3:3">
       <c r="C75" s="14"/>
     </row>
-    <row r="76" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A76" s="7">
-        <v>74</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>49</v>
-      </c>
+    <row r="76" ht="14" customHeight="1" spans="3:3">
       <c r="C76" s="14"/>
     </row>
-    <row r="77" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A77" s="7">
-        <v>75</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>60</v>
-      </c>
+    <row r="77" ht="14" customHeight="1" spans="3:3">
       <c r="C77" s="14"/>
     </row>
-    <row r="78" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A78" s="7">
-        <v>76</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>38</v>
-      </c>
+    <row r="78" ht="14" customHeight="1" spans="3:3">
       <c r="C78" s="14"/>
     </row>
-    <row r="79" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A79" s="7">
-        <v>77</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>80</v>
-      </c>
+    <row r="79" ht="14" customHeight="1" spans="3:3">
       <c r="C79" s="14"/>
     </row>
-    <row r="80" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A80" s="7">
-        <v>78</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>24</v>
-      </c>
+    <row r="80" ht="14" customHeight="1" spans="3:3">
       <c r="C80" s="14"/>
     </row>
-    <row r="81" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A81" s="7">
-        <v>79</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>32</v>
-      </c>
+    <row r="81" ht="14" customHeight="1" spans="3:3">
       <c r="C81" s="14"/>
     </row>
-    <row r="82" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A82" s="7">
-        <v>80</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>76</v>
-      </c>
+    <row r="82" ht="14" customHeight="1" spans="3:3">
       <c r="C82" s="14"/>
     </row>
-    <row r="83" ht="14.1" customHeight="1" spans="1:3">
-      <c r="A83" s="7">
-        <v>81</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>66</v>
-      </c>
+    <row r="83" ht="14" customHeight="1" spans="3:3">
       <c r="C83" s="14"/>
     </row>
-    <row r="84" ht="14.1" customHeight="1" spans="3:3">
+    <row r="84" ht="14" customHeight="1" spans="3:3">
       <c r="C84" s="14"/>
     </row>
-    <row r="85" ht="14.1" customHeight="1" spans="3:3">
+    <row r="85" ht="14" customHeight="1" spans="3:3">
       <c r="C85" s="14"/>
     </row>
-    <row r="86" ht="14.1" customHeight="1" spans="3:3">
+    <row r="86" ht="14" customHeight="1" spans="3:3">
       <c r="C86" s="14"/>
     </row>
     <row r="87" ht="14.1" customHeight="1" spans="3:3">
@@ -4655,21 +4418,4 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="72"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>